<commit_message>
Se arregla interfaz dicha por Diego Lopez
</commit_message>
<xml_diff>
--- a/datos/baseDatos.xlsx
+++ b/datos/baseDatos.xlsx
@@ -413,63 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>cristian gallego</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>3117077453</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>jnm</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>